<commit_message>
* Final fixes of code refactoring and test adjustments. * Added the implementation of duplicate handling for external sorts.
</commit_message>
<xml_diff>
--- a/tests/data/desired/dataformatreport.xlsx
+++ b/tests/data/desired/dataformatreport.xlsx
@@ -49,7 +49,7 @@
     <numFmt numFmtId="168" formatCode="HH:MM AM/PM"/>
     <numFmt numFmtId="169" formatCode="0,00E+00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -62,10 +62,34 @@
       <sz val="11.0"/>
       <b val="true"/>
       <color indexed="8"/>
-      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,15 +97,12 @@
       <patternFill patternType="darkGray"/>
     </fill>
     <fill>
-      <patternFill patternType="solid"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
+      <patternFill>
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill>
+      <patternFill patternType="solid">
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
@@ -91,7 +112,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="none">
         <fgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -108,15 +129,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="168" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
+    <xf numFmtId="169" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -139,485 +159,485 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" t="s" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="3">
+      <c r="A2" t="n" s="2">
         <v>0.0</v>
       </c>
-      <c r="B2" t="n" s="4">
+      <c r="B2" t="n" s="3">
         <v>40897.458333333336</v>
       </c>
-      <c r="C2" t="n" s="5">
+      <c r="C2" t="n" s="4">
         <v>40848.0</v>
       </c>
-      <c r="D2" t="n" s="6">
+      <c r="D2" t="n" s="5">
         <v>25569.0</v>
       </c>
-      <c r="E2" t="n" s="3">
+      <c r="E2" t="n" s="2">
         <v>0.0</v>
       </c>
-      <c r="F2" t="n" s="7">
+      <c r="F2" t="n" s="6">
         <v>0.0</v>
       </c>
-      <c r="G2" t="n" s="3">
+      <c r="G2" t="n" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="3">
+      <c r="A3" t="n" s="2">
         <v>1.0</v>
       </c>
-      <c r="B3" t="n" s="4">
+      <c r="B3" t="n" s="3">
         <v>40897.45903935185</v>
       </c>
-      <c r="C3" t="n" s="5">
+      <c r="C3" t="n" s="4">
         <v>40849.0</v>
       </c>
-      <c r="D3" t="n" s="6">
+      <c r="D3" t="n" s="5">
         <v>25569.042372685184</v>
       </c>
-      <c r="E3" t="n" s="3">
+      <c r="E3" t="n" s="2">
         <v>2.0</v>
       </c>
-      <c r="F3" t="n" s="7">
+      <c r="F3" t="n" s="6">
         <v>1.0</v>
       </c>
-      <c r="G3" t="n" s="3">
+      <c r="G3" t="n" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="3">
+      <c r="A4" t="n" s="2">
         <v>2.0</v>
       </c>
-      <c r="B4" t="n" s="4">
+      <c r="B4" t="n" s="3">
         <v>40897.45974537037</v>
       </c>
-      <c r="C4" t="n" s="5">
+      <c r="C4" t="n" s="4">
         <v>40850.0</v>
       </c>
-      <c r="D4" t="n" s="6">
+      <c r="D4" t="n" s="5">
         <v>25569.084745370372</v>
       </c>
-      <c r="E4" t="n" s="3">
+      <c r="E4" t="n" s="2">
         <v>4.0</v>
       </c>
-      <c r="F4" t="n" s="7">
+      <c r="F4" t="n" s="6">
         <v>4.0</v>
       </c>
-      <c r="G4" t="n" s="3">
+      <c r="G4" t="n" s="2">
         <v>6.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="3">
+      <c r="A5" t="n" s="2">
         <v>3.0</v>
       </c>
-      <c r="B5" t="n" s="4">
+      <c r="B5" t="n" s="3">
         <v>40897.46045138889</v>
       </c>
-      <c r="C5" t="n" s="5">
+      <c r="C5" t="n" s="4">
         <v>40851.0</v>
       </c>
-      <c r="D5" t="n" s="6">
+      <c r="D5" t="n" s="5">
         <v>25569.127118055556</v>
       </c>
-      <c r="E5" t="n" s="3">
+      <c r="E5" t="n" s="2">
         <v>6.0</v>
       </c>
-      <c r="F5" t="n" s="7">
+      <c r="F5" t="n" s="6">
         <v>9.0</v>
       </c>
-      <c r="G5" t="n" s="3">
+      <c r="G5" t="n" s="2">
         <v>12.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="3">
+      <c r="A6" t="n" s="2">
         <v>4.0</v>
       </c>
-      <c r="B6" t="n" s="4">
+      <c r="B6" t="n" s="3">
         <v>40897.46115740741</v>
       </c>
-      <c r="C6" t="n" s="5">
+      <c r="C6" t="n" s="4">
         <v>40852.0</v>
       </c>
-      <c r="D6" t="n" s="6">
+      <c r="D6" t="n" s="5">
         <v>25569.16949074074</v>
       </c>
-      <c r="E6" t="n" s="3">
+      <c r="E6" t="n" s="2">
         <v>8.0</v>
       </c>
-      <c r="F6" t="n" s="7">
+      <c r="F6" t="n" s="6">
         <v>16.0</v>
       </c>
-      <c r="G6" t="n" s="3">
+      <c r="G6" t="n" s="2">
         <v>20.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="3">
+      <c r="A7" t="n" s="2">
         <v>5.0</v>
       </c>
-      <c r="B7" t="n" s="4">
+      <c r="B7" t="n" s="3">
         <v>40897.461863425924</v>
       </c>
-      <c r="C7" t="n" s="5">
+      <c r="C7" t="n" s="4">
         <v>40853.0</v>
       </c>
-      <c r="D7" t="n" s="6">
+      <c r="D7" t="n" s="5">
         <v>25569.211863425928</v>
       </c>
-      <c r="E7" t="n" s="3">
+      <c r="E7" t="n" s="2">
         <v>10.0</v>
       </c>
-      <c r="F7" t="n" s="7">
+      <c r="F7" t="n" s="6">
         <v>25.0</v>
       </c>
-      <c r="G7" t="n" s="3">
+      <c r="G7" t="n" s="2">
         <v>30.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="3">
+      <c r="A8" t="n" s="2">
         <v>6.0</v>
       </c>
-      <c r="B8" t="n" s="4">
+      <c r="B8" t="n" s="3">
         <v>40897.46256944445</v>
       </c>
-      <c r="C8" t="n" s="5">
+      <c r="C8" t="n" s="4">
         <v>40854.0</v>
       </c>
-      <c r="D8" t="n" s="6">
+      <c r="D8" t="n" s="5">
         <v>25569.254236111112</v>
       </c>
-      <c r="E8" t="n" s="3">
+      <c r="E8" t="n" s="2">
         <v>12.0</v>
       </c>
-      <c r="F8" t="n" s="7">
+      <c r="F8" t="n" s="6">
         <v>36.0</v>
       </c>
-      <c r="G8" t="n" s="3">
+      <c r="G8" t="n" s="2">
         <v>42.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="3">
+      <c r="A9" t="n" s="2">
         <v>7.0</v>
       </c>
-      <c r="B9" t="n" s="4">
+      <c r="B9" t="n" s="3">
         <v>40897.463275462964</v>
       </c>
-      <c r="C9" t="n" s="5">
+      <c r="C9" t="n" s="4">
         <v>40855.0</v>
       </c>
-      <c r="D9" t="n" s="6">
+      <c r="D9" t="n" s="5">
         <v>25569.296608796296</v>
       </c>
-      <c r="E9" t="n" s="3">
+      <c r="E9" t="n" s="2">
         <v>14.0</v>
       </c>
-      <c r="F9" t="n" s="7">
+      <c r="F9" t="n" s="6">
         <v>49.0</v>
       </c>
-      <c r="G9" t="n" s="3">
+      <c r="G9" t="n" s="2">
         <v>56.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="3">
+      <c r="A10" t="n" s="2">
         <v>8.0</v>
       </c>
-      <c r="B10" t="n" s="4">
+      <c r="B10" t="n" s="3">
         <v>40897.46398148148</v>
       </c>
-      <c r="C10" t="n" s="5">
+      <c r="C10" t="n" s="4">
         <v>40856.0</v>
       </c>
-      <c r="D10" t="n" s="6">
+      <c r="D10" t="n" s="5">
         <v>25569.33898148148</v>
       </c>
-      <c r="E10" t="n" s="3">
+      <c r="E10" t="n" s="2">
         <v>16.0</v>
       </c>
-      <c r="F10" t="n" s="7">
+      <c r="F10" t="n" s="6">
         <v>64.0</v>
       </c>
-      <c r="G10" t="n" s="3">
+      <c r="G10" t="n" s="2">
         <v>72.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="3">
+      <c r="A11" t="n" s="2">
         <v>9.0</v>
       </c>
-      <c r="B11" t="n" s="4">
+      <c r="B11" t="n" s="3">
         <v>40897.4646875</v>
       </c>
-      <c r="C11" t="n" s="5">
+      <c r="C11" t="n" s="4">
         <v>40857.0</v>
       </c>
-      <c r="D11" t="n" s="6">
+      <c r="D11" t="n" s="5">
         <v>25569.381354166668</v>
       </c>
-      <c r="E11" t="n" s="3">
+      <c r="E11" t="n" s="2">
         <v>18.0</v>
       </c>
-      <c r="F11" t="n" s="7">
+      <c r="F11" t="n" s="6">
         <v>81.0</v>
       </c>
-      <c r="G11" t="n" s="3">
+      <c r="G11" t="n" s="2">
         <v>90.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="3">
+      <c r="A12" t="n" s="2">
         <v>10.0</v>
       </c>
-      <c r="B12" t="n" s="4">
+      <c r="B12" t="n" s="3">
         <v>40897.46539351852</v>
       </c>
-      <c r="C12" t="n" s="5">
+      <c r="C12" t="n" s="4">
         <v>40858.0</v>
       </c>
-      <c r="D12" t="n" s="6">
+      <c r="D12" t="n" s="5">
         <v>25569.423726851852</v>
       </c>
-      <c r="E12" t="n" s="3">
+      <c r="E12" t="n" s="2">
         <v>20.0</v>
       </c>
-      <c r="F12" t="n" s="7">
+      <c r="F12" t="n" s="6">
         <v>100.0</v>
       </c>
-      <c r="G12" t="n" s="3">
+      <c r="G12" t="n" s="2">
         <v>110.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n" s="3">
+      <c r="A13" t="n" s="2">
         <v>11.0</v>
       </c>
-      <c r="B13" t="n" s="4">
+      <c r="B13" t="n" s="3">
         <v>40897.466099537036</v>
       </c>
-      <c r="C13" t="n" s="5">
+      <c r="C13" t="n" s="4">
         <v>40859.0</v>
       </c>
-      <c r="D13" t="n" s="6">
+      <c r="D13" t="n" s="5">
         <v>25569.466099537036</v>
       </c>
-      <c r="E13" t="n" s="3">
+      <c r="E13" t="n" s="2">
         <v>22.0</v>
       </c>
-      <c r="F13" t="n" s="7">
+      <c r="F13" t="n" s="6">
         <v>121.0</v>
       </c>
-      <c r="G13" t="n" s="3">
+      <c r="G13" t="n" s="2">
         <v>132.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="3">
+      <c r="A14" t="n" s="2">
         <v>12.0</v>
       </c>
-      <c r="B14" t="n" s="4">
+      <c r="B14" t="n" s="3">
         <v>40897.46680555555</v>
       </c>
-      <c r="C14" t="n" s="5">
+      <c r="C14" t="n" s="4">
         <v>40860.0</v>
       </c>
-      <c r="D14" t="n" s="6">
+      <c r="D14" t="n" s="5">
         <v>25569.508472222224</v>
       </c>
-      <c r="E14" t="n" s="3">
+      <c r="E14" t="n" s="2">
         <v>24.0</v>
       </c>
-      <c r="F14" t="n" s="7">
+      <c r="F14" t="n" s="6">
         <v>144.0</v>
       </c>
-      <c r="G14" t="n" s="3">
+      <c r="G14" t="n" s="2">
         <v>156.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="3">
+      <c r="A15" t="n" s="2">
         <v>13.0</v>
       </c>
-      <c r="B15" t="n" s="4">
+      <c r="B15" t="n" s="3">
         <v>40897.467511574076</v>
       </c>
-      <c r="C15" t="n" s="5">
+      <c r="C15" t="n" s="4">
         <v>40861.0</v>
       </c>
-      <c r="D15" t="n" s="6">
+      <c r="D15" t="n" s="5">
         <v>25569.550844907408</v>
       </c>
-      <c r="E15" t="n" s="3">
+      <c r="E15" t="n" s="2">
         <v>26.0</v>
       </c>
-      <c r="F15" t="n" s="7">
+      <c r="F15" t="n" s="6">
         <v>169.0</v>
       </c>
-      <c r="G15" t="n" s="3">
+      <c r="G15" t="n" s="2">
         <v>182.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="3">
+      <c r="A16" t="n" s="2">
         <v>14.0</v>
       </c>
-      <c r="B16" t="n" s="4">
+      <c r="B16" t="n" s="3">
         <v>40897.46821759259</v>
       </c>
-      <c r="C16" t="n" s="5">
+      <c r="C16" t="n" s="4">
         <v>40862.0</v>
       </c>
-      <c r="D16" t="n" s="6">
+      <c r="D16" t="n" s="5">
         <v>25569.593217592592</v>
       </c>
-      <c r="E16" t="n" s="3">
+      <c r="E16" t="n" s="2">
         <v>28.0</v>
       </c>
-      <c r="F16" t="n" s="7">
+      <c r="F16" t="n" s="6">
         <v>196.0</v>
       </c>
-      <c r="G16" t="n" s="3">
+      <c r="G16" t="n" s="2">
         <v>210.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="3">
+      <c r="A17" t="n" s="2">
         <v>15.0</v>
       </c>
-      <c r="B17" t="n" s="4">
+      <c r="B17" t="n" s="3">
         <v>40897.46892361111</v>
       </c>
-      <c r="C17" t="n" s="5">
+      <c r="C17" t="n" s="4">
         <v>40863.0</v>
       </c>
-      <c r="D17" t="n" s="6">
+      <c r="D17" t="n" s="5">
         <v>25569.63559027778</v>
       </c>
-      <c r="E17" t="n" s="3">
+      <c r="E17" t="n" s="2">
         <v>30.0</v>
       </c>
-      <c r="F17" t="n" s="7">
+      <c r="F17" t="n" s="6">
         <v>225.0</v>
       </c>
-      <c r="G17" t="n" s="3">
+      <c r="G17" t="n" s="2">
         <v>240.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="3">
+      <c r="A18" t="n" s="2">
         <v>16.0</v>
       </c>
-      <c r="B18" t="n" s="4">
+      <c r="B18" t="n" s="3">
         <v>40897.46962962963</v>
       </c>
-      <c r="C18" t="n" s="5">
+      <c r="C18" t="n" s="4">
         <v>40864.0</v>
       </c>
-      <c r="D18" t="n" s="6">
+      <c r="D18" t="n" s="5">
         <v>25569.677962962964</v>
       </c>
-      <c r="E18" t="n" s="3">
+      <c r="E18" t="n" s="2">
         <v>32.0</v>
       </c>
-      <c r="F18" t="n" s="7">
+      <c r="F18" t="n" s="6">
         <v>256.0</v>
       </c>
-      <c r="G18" t="n" s="3">
+      <c r="G18" t="n" s="2">
         <v>272.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n" s="3">
+      <c r="A19" t="n" s="2">
         <v>17.0</v>
       </c>
-      <c r="B19" t="n" s="4">
+      <c r="B19" t="n" s="3">
         <v>40897.47033564815</v>
       </c>
-      <c r="C19" t="n" s="5">
+      <c r="C19" t="n" s="4">
         <v>40865.0</v>
       </c>
-      <c r="D19" t="n" s="6">
+      <c r="D19" t="n" s="5">
         <v>25569.720335648148</v>
       </c>
-      <c r="E19" t="n" s="3">
+      <c r="E19" t="n" s="2">
         <v>34.0</v>
       </c>
-      <c r="F19" t="n" s="7">
+      <c r="F19" t="n" s="6">
         <v>289.0</v>
       </c>
-      <c r="G19" t="n" s="3">
+      <c r="G19" t="n" s="2">
         <v>306.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n" s="3">
+      <c r="A20" t="n" s="2">
         <v>18.0</v>
       </c>
-      <c r="B20" t="n" s="4">
+      <c r="B20" t="n" s="3">
         <v>40897.471041666664</v>
       </c>
-      <c r="C20" t="n" s="5">
+      <c r="C20" t="n" s="4">
         <v>40866.0</v>
       </c>
-      <c r="D20" t="n" s="6">
+      <c r="D20" t="n" s="5">
         <v>25569.762708333332</v>
       </c>
-      <c r="E20" t="n" s="3">
+      <c r="E20" t="n" s="2">
         <v>36.0</v>
       </c>
-      <c r="F20" t="n" s="7">
+      <c r="F20" t="n" s="6">
         <v>324.0</v>
       </c>
-      <c r="G20" t="n" s="3">
+      <c r="G20" t="n" s="2">
         <v>342.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="3">
+      <c r="A21" t="n" s="2">
         <v>19.0</v>
       </c>
-      <c r="B21" t="n" s="4">
+      <c r="B21" t="n" s="3">
         <v>40897.47174768519</v>
       </c>
-      <c r="C21" t="n" s="5">
+      <c r="C21" t="n" s="4">
         <v>40867.0</v>
       </c>
-      <c r="D21" t="n" s="6">
+      <c r="D21" t="n" s="5">
         <v>25569.80508101852</v>
       </c>
-      <c r="E21" t="n" s="3">
+      <c r="E21" t="n" s="2">
         <v>38.0</v>
       </c>
-      <c r="F21" t="n" s="7">
+      <c r="F21" t="n" s="6">
         <v>361.0</v>
       </c>
-      <c r="G21" t="n" s="3">
+      <c r="G21" t="n" s="2">
         <v>380.0</v>
       </c>
     </row>

</xml_diff>